<commit_message>
Actualizacion de corridas de test
</commit_message>
<xml_diff>
--- a/Producto/Web/Casos de prueba/Ejecuciones/GeoP_PlanPrueba_TestCaseExec.xlsx
+++ b/Producto/Web/Casos de prueba/Ejecuciones/GeoP_PlanPrueba_TestCaseExec.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="630" windowWidth="9015" windowHeight="7110" activeTab="3"/>
+    <workbookView xWindow="510" yWindow="630" windowWidth="9015" windowHeight="7110" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TC_01" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="TC_11" sheetId="9" r:id="rId9"/>
     <sheet name="TC_12" sheetId="10" r:id="rId10"/>
     <sheet name="TC_13" sheetId="11" r:id="rId11"/>
+    <sheet name="TC_14_lucas" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="124">
   <si>
     <t>Registro de ejecución de Test Cases</t>
   </si>
@@ -381,13 +382,28 @@
   </si>
   <si>
     <t>Se carga un modal con todos los datos de la playa &lt;Playa1&gt; y no me permite modificarlos</t>
+  </si>
+  <si>
+    <t>14_lucas</t>
+  </si>
+  <si>
+    <t>ingresar "cordoba" en el nombre de la ciudad a buscar</t>
+  </si>
+  <si>
+    <t>se muestra una lista con las ciudades de google que se correspondan con "cordoba"</t>
+  </si>
+  <si>
+    <t>Selecciono la opcion "Córdoba, Argentina"</t>
+  </si>
+  <si>
+    <t>Se redirige a la pagina Busqueda.aspx y se muestra el mapa ubicado en la ciudad de Córdoba y se visualizan los marcadores de las playas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -794,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -948,10 +964,14 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,6 +1061,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1075,6 +1096,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1250,14 +1272,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -1266,28 +1288,28 @@
     <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1296,7 +1318,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1305,7 +1327,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1316,7 +1338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
@@ -1325,7 +1347,7 @@
       </c>
       <c r="D7" s="51"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>89</v>
       </c>
@@ -1334,63 +1356,63 @@
       </c>
       <c r="D8" s="51"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>91</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="51"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>92</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="51"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>93</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="51"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>94</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="51"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>95</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="51"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>96</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="51"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="51"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="51"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1" thickBot="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>98</v>
       </c>
@@ -1399,63 +1421,63 @@
       </c>
       <c r="D17" s="51"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1" thickBot="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>100</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="51"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1" thickBot="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>101</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="51"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1" thickBot="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>102</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="51"/>
     </row>
-    <row r="21" spans="2:4" ht="15.75" customHeight="1" thickBot="1">
+    <row r="21" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="51"/>
     </row>
-    <row r="22" spans="2:4" ht="15.75" customHeight="1" thickBot="1">
+    <row r="22" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>95</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="51"/>
     </row>
-    <row r="23" spans="2:4" ht="15.75" customHeight="1" thickBot="1">
+    <row r="23" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>104</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="51"/>
     </row>
-    <row r="24" spans="2:4" ht="15.75" customHeight="1" thickBot="1">
+    <row r="24" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>95</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="51"/>
     </row>
-    <row r="25" spans="2:4" ht="15.75" customHeight="1" thickBot="1">
+    <row r="25" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>105</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="51"/>
     </row>
-    <row r="26" spans="2:4" ht="15.75" customHeight="1">
+    <row r="26" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
         <v>106</v>
       </c>
@@ -1473,14 +1495,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="14" customWidth="1"/>
@@ -1490,28 +1512,28 @@
     <col min="7" max="16384" width="17.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1520,7 +1542,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1529,7 +1551,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="35" t="s">
         <v>4</v>
       </c>
@@ -1540,14 +1562,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36" t="s">
         <v>76</v>
       </c>
       <c r="C7" s="37"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
         <v>77</v>
       </c>
@@ -1556,7 +1578,7 @@
       </c>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:5" ht="39" thickBot="1">
+    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
         <v>83</v>
       </c>
@@ -1565,14 +1587,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="38" t="s">
         <v>84</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="40" t="s">
         <v>80</v>
       </c>
@@ -1581,47 +1603,47 @@
       </c>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1636,14 +1658,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="14" customWidth="1"/>
@@ -1653,28 +1675,28 @@
     <col min="7" max="16384" width="17.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1683,7 +1705,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1692,7 +1714,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>4</v>
       </c>
@@ -1703,7 +1725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
         <v>76</v>
       </c>
@@ -1711,7 +1733,7 @@
       <c r="D7" s="31"/>
       <c r="E7" s="27"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="30" t="s">
         <v>77</v>
       </c>
@@ -1721,7 +1743,7 @@
       <c r="D8" s="32"/>
       <c r="E8" s="27"/>
     </row>
-    <row r="9" spans="1:5" ht="39" thickBot="1">
+    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="30" t="s">
         <v>86</v>
       </c>
@@ -1729,7 +1751,7 @@
       <c r="D9" s="33"/>
       <c r="E9" s="27"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
         <v>80</v>
       </c>
@@ -1739,52 +1761,52 @@
       <c r="D10" s="34"/>
       <c r="E10" s="27"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1798,15 +1820,126 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="62.28515625" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="61"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="61"/>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="61"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="61"/>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42051</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="61"/>
+      <c r="B6" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61"/>
+      <c r="B7" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="61"/>
+      <c r="B8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61"/>
+      <c r="B9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="61"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
@@ -1815,28 +1948,28 @@
     <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1845,7 +1978,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1854,7 +1987,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
@@ -1865,7 +1998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
@@ -1874,14 +2007,14 @@
       </c>
       <c r="D7" s="51"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="51"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>45</v>
       </c>
@@ -1890,7 +2023,7 @@
       </c>
       <c r="D9" s="51"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>47</v>
       </c>
@@ -1899,14 +2032,14 @@
       </c>
       <c r="D10" s="51"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>110</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="51"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>54</v>
       </c>
@@ -1915,7 +2048,7 @@
       </c>
       <c r="D12" s="51"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>56</v>
       </c>
@@ -1924,37 +2057,37 @@
       </c>
       <c r="D13" s="51"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="47"/>
       <c r="C14" s="57"/>
       <c r="D14" s="56"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1968,14 +2101,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
@@ -1984,28 +2117,28 @@
     <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -2014,7 +2147,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
@@ -2023,7 +2156,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
@@ -2034,7 +2167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>112</v>
       </c>
@@ -2043,14 +2176,14 @@
       </c>
       <c r="D7" s="51"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="51"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>45</v>
       </c>
@@ -2059,7 +2192,7 @@
       </c>
       <c r="D9" s="51"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>114</v>
       </c>
@@ -2068,7 +2201,7 @@
       </c>
       <c r="D10" s="51"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>56</v>
       </c>
@@ -2077,47 +2210,47 @@
       </c>
       <c r="D11" s="51"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="53"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="47"/>
       <c r="C13" s="58"/>
       <c r="D13" s="21"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="47"/>
       <c r="C14" s="58"/>
       <c r="D14" s="21"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="47"/>
       <c r="C15" s="50"/>
       <c r="D15" s="21"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2131,14 +2264,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
@@ -2147,28 +2280,28 @@
     <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
@@ -2177,7 +2310,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
@@ -2186,7 +2319,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
@@ -2197,7 +2330,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
@@ -2206,14 +2339,14 @@
       </c>
       <c r="D7" s="55"/>
     </row>
-    <row r="8" spans="1:5" ht="12.75" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="55"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>45</v>
       </c>
@@ -2222,7 +2355,7 @@
       </c>
       <c r="D9" s="55"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>47</v>
       </c>
@@ -2231,7 +2364,7 @@
       </c>
       <c r="D10" s="55"/>
     </row>
-    <row r="11" spans="1:5" ht="30.75" customHeight="1" thickBot="1">
+    <row r="11" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>49</v>
       </c>
@@ -2242,21 +2375,21 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="55"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="55"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>52</v>
       </c>
@@ -2265,7 +2398,7 @@
       </c>
       <c r="D14" s="55"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>54</v>
       </c>
@@ -2274,7 +2407,7 @@
       </c>
       <c r="D15" s="55"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>56</v>
       </c>
@@ -2283,7 +2416,7 @@
       </c>
       <c r="D16" s="55"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2297,14 +2430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
@@ -2313,28 +2446,28 @@
     <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
@@ -2343,7 +2476,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
@@ -2352,7 +2485,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="35" t="s">
         <v>32</v>
       </c>
@@ -2363,7 +2496,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
@@ -2372,14 +2505,14 @@
       </c>
       <c r="D7" s="55"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="55"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>45</v>
       </c>
@@ -2388,7 +2521,7 @@
       </c>
       <c r="D9" s="55"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
         <v>117</v>
       </c>
@@ -2397,57 +2530,57 @@
       </c>
       <c r="D10" s="55"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="59"/>
       <c r="C11" s="60"/>
       <c r="D11" s="22"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="47"/>
       <c r="C12" s="48"/>
       <c r="D12" s="22"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="47"/>
       <c r="C13" s="48"/>
       <c r="D13" s="22"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="47"/>
       <c r="C14" s="49"/>
       <c r="D14" s="22"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="47"/>
       <c r="C15" s="50"/>
       <c r="D15" s="22"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="15.75" customHeight="1">
+    <row r="21" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
     </row>
@@ -2460,14 +2593,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
@@ -2476,28 +2609,28 @@
     <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
@@ -2506,7 +2639,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
@@ -2515,7 +2648,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
@@ -2526,21 +2659,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="55"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="55"/>
     </row>
-    <row r="9" spans="1:5" ht="39" thickBot="1">
+    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>45</v>
       </c>
@@ -2551,57 +2684,57 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="55"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="47"/>
       <c r="C12" s="48"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="47"/>
       <c r="C13" s="48"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="47"/>
       <c r="C14" s="49"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="47"/>
       <c r="C15" s="50"/>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2615,14 +2748,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="11" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="11" customWidth="1"/>
@@ -2632,28 +2765,28 @@
     <col min="7" max="16384" width="17.28515625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2662,7 +2795,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2671,7 +2804,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
@@ -2682,21 +2815,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="51"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>60</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="51"/>
     </row>
-    <row r="9" spans="1:5" ht="39" thickBot="1">
+    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>45</v>
       </c>
@@ -2707,56 +2840,56 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="51"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="51"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="51"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="51"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="51"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="51"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="51"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="13" t="s">
         <v>70</v>
       </c>
@@ -2765,17 +2898,17 @@
       </c>
       <c r="D17" s="51"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2789,14 +2922,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="11" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="11" customWidth="1"/>
@@ -2806,28 +2939,28 @@
     <col min="7" max="16384" width="17.28515625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2836,7 +2969,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2845,7 +2978,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
@@ -2856,21 +2989,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="51"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>60</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="51"/>
     </row>
-    <row r="9" spans="1:5" ht="39" thickBot="1">
+    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>45</v>
       </c>
@@ -2881,21 +3014,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="51"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="51"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="s">
         <v>45</v>
       </c>
@@ -2906,42 +3039,42 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2955,14 +3088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="14" customWidth="1"/>
@@ -2972,28 +3105,28 @@
     <col min="7" max="16384" width="17.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3002,7 +3135,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3011,7 +3144,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="35" t="s">
         <v>4</v>
       </c>
@@ -3022,14 +3155,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36" t="s">
         <v>76</v>
       </c>
       <c r="C7" s="43"/>
       <c r="D7" s="25"/>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
         <v>77</v>
       </c>
@@ -3038,7 +3171,7 @@
       </c>
       <c r="D8" s="26"/>
     </row>
-    <row r="9" spans="1:5" ht="39" thickBot="1">
+    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
         <v>79</v>
       </c>
@@ -3047,7 +3180,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
         <v>80</v>
       </c>
@@ -3056,52 +3189,52 @@
       </c>
       <c r="D10" s="26"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>

</xml_diff>

<commit_message>
Actualizacion corrida de test
</commit_message>
<xml_diff>
--- a/Producto/Web/Casos de prueba/Ejecuciones/GeoP_PlanPrueba_TestCaseExec.xlsx
+++ b/Producto/Web/Casos de prueba/Ejecuciones/GeoP_PlanPrueba_TestCaseExec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="630" windowWidth="9015" windowHeight="7110" activeTab="11"/>
+    <workbookView xWindow="510" yWindow="630" windowWidth="9015" windowHeight="7110" tabRatio="665" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TC_01" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="TC_12" sheetId="10" r:id="rId10"/>
     <sheet name="TC_13" sheetId="11" r:id="rId11"/>
     <sheet name="TC_14_lucas" sheetId="12" r:id="rId12"/>
+    <sheet name="TC_15_lucas" sheetId="13" r:id="rId13"/>
+    <sheet name="TC_16_lucas" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
   <si>
     <t>Registro de ejecución de Test Cases</t>
   </si>
@@ -397,6 +399,48 @@
   </si>
   <si>
     <t>Se redirige a la pagina Busqueda.aspx y se muestra el mapa ubicado en la ciudad de Córdoba y se visualizan los marcadores de las playas.</t>
+  </si>
+  <si>
+    <t>ingresar "jesus maria" en el nombre de la ciudad a buscar</t>
+  </si>
+  <si>
+    <t>se muestra una lista con las ciudades de google que se correspondan con "jesus maria"</t>
+  </si>
+  <si>
+    <t>Selecciono la opcion "Jesús María, Córdoba, Argentina"</t>
+  </si>
+  <si>
+    <t>Se redirige a la pagina Busqueda.aspx y se muestra el mapa ubicado en la ciudad de Jesús María y se visualiza un mensaje de que no hay playas cargadas en esa ciudad.</t>
+  </si>
+  <si>
+    <t>ingreso al sitio web.</t>
+  </si>
+  <si>
+    <t>Escribo "jesus maria" en donde se debe ingresar la ciudad a buscar.</t>
+  </si>
+  <si>
+    <t>Se muestra el autocomplete con las opciones de las ciudad que se corresponden con la cadena "jesus maria".</t>
+  </si>
+  <si>
+    <t>Selecciono "Jesús María, Córdoba, Argentina" en la lista de ciudad del autocomplete y presiono BUSCAR</t>
+  </si>
+  <si>
+    <t>Me redirige a la pagina "BusquedaPlayas.aspx" y se muestra en el mapa la ciudad de Jesús María y las playas de esa ciudad</t>
+  </si>
+  <si>
+    <t>En la seccion de busqueda avanzada, selecciono como filtro un tipo de vehiculo (Auto)</t>
+  </si>
+  <si>
+    <t>Se crea el tags de filtro correspondiente al tipo de vehiculo Auto</t>
+  </si>
+  <si>
+    <t>Presiono Filtrar</t>
+  </si>
+  <si>
+    <t>Se muestran en el mapa solo las playas que tengan dentro de sus servicios, el correspondiente al tipo de vehiculo "Auto"</t>
+  </si>
+  <si>
+    <t>16_lucas</t>
   </si>
 </sst>
 </file>
@@ -412,106 +456,126 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="36"/>
       <color rgb="FF38761D"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -810,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -965,13 +1029,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,12 +1354,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1513,12 +1578,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1676,12 +1741,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1824,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1836,12 +1901,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="61"/>
@@ -1862,7 +1927,7 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="63" t="s">
         <v>119</v>
       </c>
       <c r="D4" s="1"/>
@@ -1922,6 +1987,241 @@
       <c r="B10" s="30"/>
       <c r="C10" s="29"/>
       <c r="D10" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="62"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="62"/>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="62"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="62"/>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42051</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="62"/>
+      <c r="B6" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="62"/>
+      <c r="B7" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="62"/>
+      <c r="B8" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="62"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" customWidth="1"/>
+    <col min="4" max="4" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="62"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="62"/>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="62"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="62"/>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42047</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="62"/>
+      <c r="B6" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="62"/>
+      <c r="B7" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="62"/>
+      <c r="B8" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="62"/>
+      <c r="B10" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1949,12 +2249,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2118,12 +2418,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2281,12 +2581,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2447,12 +2747,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2610,12 +2910,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2766,12 +3066,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2940,12 +3240,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3106,12 +3406,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>